<commit_message>
전투 ui 제작 // ui
</commit_message>
<xml_diff>
--- a/기획문서/중간발표/일정엑셀.xlsx
+++ b/기획문서/중간발표/일정엑셀.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16828"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Aww\기획문서\중간발표\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="96" windowWidth="27792" windowHeight="12336"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,8 +164,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,8 +197,25 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,7 +252,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,75 +400,81 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="2" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="2" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="나쁨" xfId="2" builtinId="27"/>
-    <cellStyle name="좋음" xfId="1" builtinId="26"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,7 +490,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -502,7 +532,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,26 +565,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,23 +600,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -782,17 +778,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -824,94 +820,94 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="2"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" s="15"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="4"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" s="15"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" s="15"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" s="15"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" s="15"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="2"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" s="15"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
@@ -920,12 +916,12 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9" s="15"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -933,13 +929,13 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A10" s="16"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
@@ -947,69 +943,69 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A11" s="8" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="4"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A12" s="9"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="4"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="2"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A13" s="9"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="5"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A14" s="9"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="5"/>
+      <c r="H14" s="21"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A15" s="10"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1017,71 +1013,71 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A16" s="11" t="s">
+      <c r="G15" s="3"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="4"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="2"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="4"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="2"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A18" s="12"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="4"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="2"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="4"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="2"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A20" s="12"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1089,13 +1085,13 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="5"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A21" s="12"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1103,13 +1099,13 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="3"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="22"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A22" s="13"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1117,81 +1113,81 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="G22" s="3"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="4"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="2"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="2"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="G26" s="3"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
       <c r="J27" s="1"/>
     </row>
   </sheetData>
@@ -1213,7 +1209,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1226,7 +1222,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>